<commit_message>
Latest code as of 27th April 11:25 AM having latest Hashmap Changes against TC004 and TC003
</commit_message>
<xml_diff>
--- a/src/test/java/com/automation/testData/TestData.xlsx
+++ b/src/test/java/com/automation/testData/TestData.xlsx
@@ -1,33 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\AutomationTesting\src\test\java\com\automation\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12828" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12825" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -84,13 +73,55 @@
   </si>
   <si>
     <t>tUdegar</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>passWord</t>
+  </si>
+  <si>
+    <t>setCustName</t>
+  </si>
+  <si>
+    <t>setCustGender</t>
+  </si>
+  <si>
+    <t>setCustDob</t>
+  </si>
+  <si>
+    <t>setCustAdd</t>
+  </si>
+  <si>
+    <t>setCustCity</t>
+  </si>
+  <si>
+    <t>setCustState</t>
+  </si>
+  <si>
+    <t>setCustPin</t>
+  </si>
+  <si>
+    <t>setCustMob</t>
+  </si>
+  <si>
+    <t>setCustPass</t>
+  </si>
+  <si>
+    <t>Ashutosh</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>Vatika G21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -162,6 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -223,7 +255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,10 +287,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,7 +321,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,33 +496,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6">
+        <v>32826</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>122004</v>
+      </c>
+      <c r="J2">
+        <v>9953229953</v>
+      </c>
+      <c r="K2">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -501,97 +593,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>32826</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>122002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>1234567890</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -603,12 +695,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>